<commit_message>
updated Articles GDrive URLs
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\charlottepizarras.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charlotte Pizarras\Documents\charlottepizarras.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1571654A-14AB-44D2-AC9D-466981B08151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE139F74-3BE9-4237-A342-B2C5D35F74AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29925" yWindow="1125" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="402">
   <si>
     <t>category</t>
   </si>
@@ -1162,12 +1162,6 @@
     <t>CORAL RESTORATION IN MARINDUQUE SEEN TO IMPROVE PRODUCTIVITY OF MARINE RESOURCES</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1gDnAZMctL5p9RECrUUzC6m2p8q6YkVuP/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/1mnJHmzZ0uBsaE3URHMtPdt6kfnUEj4NM/view?usp=sharing</t>
-  </si>
-  <si>
     <t>Safe water for Palawan island assured</t>
   </si>
   <si>
@@ -1183,13 +1177,7 @@
     <t>MinSU leads in calamansi research</t>
   </si>
   <si>
-    <t>https://drive.google.com/file/d/1AfMaBN70wepX_TwY9OOZ5Kw6r9RftlDK/view?usp=sharing</t>
-  </si>
-  <si>
     <t>https://drive.google.com/file/d/1J62r0r_x9MtJ09snT_QO9F2KeeXVZe2B/view?usp=sharing</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/file/d/17THWbERvifm5G_Vn6nU2pB6DasYEdI5W/view?usp=sharing</t>
   </si>
   <si>
     <t>https://drive.google.com/file/d/1v49JP62CN1vCMNpk-kgmR1cz2oUxUNEn/view?usp=sharing</t>
@@ -1363,7 +1351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1392,9 +1380,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1404,13 +1389,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -1419,16 +1404,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -1715,14 +1694,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
     <col min="2" max="2" width="8.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="4"/>
@@ -1731,7 +1710,7 @@
     <col min="8" max="8" width="25.7109375" style="9" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="3" customWidth="1"/>
     <col min="10" max="10" width="25.7109375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" style="12" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="11" customWidth="1"/>
     <col min="12" max="12" width="25.7109375" style="7" customWidth="1"/>
     <col min="13" max="13" width="25.7109375" style="3" customWidth="1"/>
     <col min="14" max="14" width="50.7109375" style="6" customWidth="1"/>
@@ -1769,7 +1748,7 @@
       <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>158</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -1783,7 +1762,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="22">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1804,17 +1783,17 @@
       <c r="J2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="L2" s="19"/>
-      <c r="M2" s="10"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="4"/>
       <c r="N2" s="6" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1838,15 +1817,15 @@
       <c r="J3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="18" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="22">
+      <c r="A4" s="18">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1867,15 +1846,15 @@
       <c r="J4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="18" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1899,15 +1878,15 @@
       <c r="J5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="18" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="18">
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1925,15 +1904,15 @@
       <c r="I6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="L6" s="19" t="s">
+      <c r="L6" s="18" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22">
+      <c r="A7" s="18">
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1951,15 +1930,15 @@
       <c r="I7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="L7" s="19" t="s">
+      <c r="L7" s="18" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22">
+      <c r="A8" s="18">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1977,15 +1956,15 @@
       <c r="I8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="14" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -2003,15 +1982,15 @@
       <c r="I9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="13" t="s">
         <v>190</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="14" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22">
+      <c r="A10" s="18">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -2032,15 +2011,15 @@
       <c r="I10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="14" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22">
+      <c r="A11" s="18">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2058,15 +2037,15 @@
       <c r="I11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="14" t="s">
+      <c r="K11" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="14" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22">
+      <c r="A12" s="18">
         <v>17</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -2084,15 +2063,15 @@
       <c r="I12" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="14" t="s">
+      <c r="K12" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="14" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22">
+      <c r="A13" s="18">
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -2113,15 +2092,15 @@
       <c r="I13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K13" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="14" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22">
+      <c r="A14" s="18">
         <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -2139,15 +2118,15 @@
       <c r="I14" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="K14" s="14" t="s">
+      <c r="K14" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="14" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="18">
         <v>38</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -2165,15 +2144,15 @@
       <c r="I15" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="K15" s="14" t="s">
+      <c r="K15" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="L15" s="19" t="s">
+      <c r="L15" s="18" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="22">
+      <c r="A16" s="18">
         <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -2191,15 +2170,15 @@
       <c r="I16" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="K16" s="14" t="s">
+      <c r="K16" s="13" t="s">
         <v>196</v>
       </c>
-      <c r="L16" s="19" t="s">
+      <c r="L16" s="18" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="A17" s="18">
         <v>40</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -2214,15 +2193,15 @@
       <c r="F17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="L17" s="18" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22">
+      <c r="A18" s="18">
         <v>41</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -2240,15 +2219,15 @@
       <c r="G18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="K18" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="L18" s="19" t="s">
+      <c r="L18" s="18" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22">
+      <c r="A19" s="18">
         <v>5</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -2266,15 +2245,15 @@
       <c r="I19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="K19" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="14" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22">
+      <c r="A20" s="18">
         <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -2292,15 +2271,15 @@
       <c r="I20" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K20" s="14" t="s">
+      <c r="K20" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="L20" s="14" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22">
+      <c r="A21" s="18">
         <v>14</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -2321,15 +2300,15 @@
       <c r="J21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="K21" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="L21" s="15" t="s">
+      <c r="L21" s="14" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22">
+      <c r="A22" s="18">
         <v>15</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -2350,15 +2329,15 @@
       <c r="J22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K22" s="14" t="s">
+      <c r="K22" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="L22" s="15" t="s">
+      <c r="L22" s="14" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="22">
+      <c r="A23" s="18">
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -2376,15 +2355,15 @@
       <c r="I23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="K23" s="14" t="s">
+      <c r="K23" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="L23" s="15" t="s">
+      <c r="L23" s="14" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22">
+      <c r="A24" s="18">
         <v>20</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -2405,15 +2384,15 @@
       <c r="I24" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K24" s="14" t="s">
+      <c r="K24" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="L24" s="15" t="s">
+      <c r="L24" s="14" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22">
+      <c r="A25" s="18">
         <v>21</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -2431,15 +2410,15 @@
       <c r="I25" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K25" s="14" t="s">
+      <c r="K25" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="L25" s="15" t="s">
+      <c r="L25" s="14" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
+      <c r="A26" s="18">
         <v>11</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -2457,15 +2436,15 @@
       <c r="I26" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="K26" s="14" t="s">
+      <c r="K26" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="L26" s="19" t="s">
+      <c r="L26" s="18" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22">
+      <c r="A27" s="18">
         <v>23</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -2483,15 +2462,15 @@
       <c r="I27" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K27" s="14" t="s">
+      <c r="K27" s="13" t="s">
         <v>172</v>
       </c>
-      <c r="L27" s="19" t="s">
+      <c r="L27" s="18" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22">
+      <c r="A28" s="18">
         <v>7</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -2512,15 +2491,15 @@
       <c r="I28" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K28" s="14" t="s">
+      <c r="K28" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="L28" s="15" t="s">
+      <c r="L28" s="14" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22">
+      <c r="A29" s="18">
         <v>12</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2538,15 +2517,15 @@
       <c r="I29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K29" s="14" t="s">
+      <c r="K29" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="L29" s="15" t="s">
+      <c r="L29" s="14" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22">
+      <c r="A30" s="18">
         <v>24</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -2564,15 +2543,15 @@
       <c r="I30" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="K30" s="14" t="s">
+      <c r="K30" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="L30" s="15" t="s">
+      <c r="L30" s="14" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="22">
+      <c r="A31" s="18">
         <v>26</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -2590,15 +2569,15 @@
       <c r="I31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K31" s="14" t="s">
+      <c r="K31" s="13" t="s">
         <v>168</v>
       </c>
-      <c r="L31" s="19" t="s">
+      <c r="L31" s="18" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="22">
+      <c r="A32" s="18">
         <v>27</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -2616,15 +2595,15 @@
       <c r="I32" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="K32" s="14" t="s">
+      <c r="K32" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="L32" s="19" t="s">
+      <c r="L32" s="18" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="22">
+      <c r="A33" s="18">
         <v>28</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -2642,15 +2621,15 @@
       <c r="I33" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="K33" s="14" t="s">
+      <c r="K33" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="L33" s="19" t="s">
+      <c r="L33" s="18" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="22">
+      <c r="A34" s="18">
         <v>29</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -2668,15 +2647,15 @@
       <c r="I34" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="K34" s="14" t="s">
+      <c r="K34" s="13" t="s">
         <v>194</v>
       </c>
-      <c r="L34" s="19" t="s">
+      <c r="L34" s="18" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="22">
+      <c r="A35" s="18">
         <v>30</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -2694,15 +2673,15 @@
       <c r="I35" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K35" s="14" t="s">
+      <c r="K35" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="L35" s="19" t="s">
+      <c r="L35" s="18" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="22">
+      <c r="A36" s="18">
         <v>31</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -2720,15 +2699,15 @@
       <c r="I36" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K36" s="14" t="s">
+      <c r="K36" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="L36" s="19" t="s">
+      <c r="L36" s="18" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="22">
+      <c r="A37" s="18">
         <v>32</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -2746,15 +2725,15 @@
       <c r="I37" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="K37" s="14" t="s">
+      <c r="K37" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="L37" s="19" t="s">
+      <c r="L37" s="18" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="22">
+      <c r="A38" s="18">
         <v>33</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -2772,15 +2751,15 @@
       <c r="I38" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="K38" s="14" t="s">
+      <c r="K38" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="L38" s="19" t="s">
+      <c r="L38" s="18" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="22">
+      <c r="A39" s="18">
         <v>34</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -2798,15 +2777,15 @@
       <c r="I39" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="K39" s="14" t="s">
+      <c r="K39" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="L39" s="19" t="s">
+      <c r="L39" s="18" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="22">
+      <c r="A40" s="18">
         <v>35</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -2824,15 +2803,15 @@
       <c r="I40" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="K40" s="14" t="s">
+      <c r="K40" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="L40" s="19" t="s">
+      <c r="L40" s="18" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="22">
+      <c r="A41" s="18">
         <v>36</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -2850,15 +2829,15 @@
       <c r="I41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K41" s="14" t="s">
+      <c r="K41" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="L41" s="19" t="s">
+      <c r="L41" s="18" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="22">
+      <c r="A42" s="18">
         <v>37</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -2876,15 +2855,15 @@
       <c r="I42" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="K42" s="14" t="s">
+      <c r="K42" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="L42" s="19" t="s">
+      <c r="L42" s="18" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A43" s="22">
+      <c r="A43" s="18">
         <v>43</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -2902,15 +2881,15 @@
       <c r="I43" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="K43" s="17" t="s">
+      <c r="K43" s="16" t="s">
         <v>248</v>
       </c>
-      <c r="L43" s="11" t="s">
+      <c r="L43" s="10" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" s="22">
+      <c r="A44" s="18">
         <v>44</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -2928,16 +2907,16 @@
       <c r="I44" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="K44" s="18" t="s">
+      <c r="K44" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="L44" s="11" t="s">
+      <c r="L44" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="M44" s="16"/>
+      <c r="M44" s="15"/>
     </row>
     <row r="45" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A45" s="22">
+      <c r="A45" s="18">
         <v>45</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -2955,15 +2934,15 @@
       <c r="I45" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="K45" s="17" t="s">
+      <c r="K45" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="L45" s="11" t="s">
+      <c r="L45" s="10" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A46" s="22">
+      <c r="A46" s="18">
         <v>46</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -2981,15 +2960,15 @@
       <c r="I46" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="K46" s="17" t="s">
+      <c r="K46" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="L46" s="11" t="s">
+      <c r="L46" s="10" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47" s="22">
+      <c r="A47" s="18">
         <v>47</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -3007,15 +2986,15 @@
       <c r="I47" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="K47" s="17" t="s">
+      <c r="K47" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="L47" s="11" t="s">
+      <c r="L47" s="10" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="120" x14ac:dyDescent="0.25">
-      <c r="A48" s="22">
+      <c r="A48" s="18">
         <v>48</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -3033,15 +3012,15 @@
       <c r="I48" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="K48" s="17" t="s">
+      <c r="K48" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="L48" s="11" t="s">
+      <c r="L48" s="10" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A49" s="22">
+      <c r="A49" s="18">
         <v>49</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -3059,15 +3038,15 @@
       <c r="I49" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="K49" s="17" t="s">
+      <c r="K49" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="L49" s="11" t="s">
+      <c r="L49" s="10" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A50" s="22">
+      <c r="A50" s="18">
         <v>51</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -3085,15 +3064,15 @@
       <c r="I50" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="K50" s="17" t="s">
+      <c r="K50" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="L50" s="11" t="s">
+      <c r="L50" s="10" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A51" s="22">
+      <c r="A51" s="18">
         <v>52</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -3111,15 +3090,15 @@
       <c r="I51" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="K51" s="17" t="s">
+      <c r="K51" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="L51" s="11" t="s">
+      <c r="L51" s="10" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="52" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A52" s="22">
+      <c r="A52" s="18">
         <v>54</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -3137,15 +3116,15 @@
       <c r="I52" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="K52" s="17" t="s">
+      <c r="K52" s="16" t="s">
         <v>259</v>
       </c>
-      <c r="L52" s="11" t="s">
+      <c r="L52" s="10" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A53" s="22">
+      <c r="A53" s="18">
         <v>55</v>
       </c>
       <c r="B53" s="3" t="s">
@@ -3163,15 +3142,15 @@
       <c r="I53" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="K53" s="17" t="s">
+      <c r="K53" s="16" t="s">
         <v>260</v>
       </c>
-      <c r="L53" s="21" t="s">
+      <c r="L53" s="19" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A54" s="22">
+      <c r="A54" s="18">
         <v>56</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -3189,15 +3168,15 @@
       <c r="I54" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="K54" s="11" t="s">
-        <v>392</v>
-      </c>
-      <c r="L54" s="11" t="s">
-        <v>393</v>
+      <c r="K54" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="L54" s="10" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A55" s="22">
+      <c r="A55" s="18">
         <v>57</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -3210,17 +3189,17 @@
         <v>156</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="K55" s="11" t="s">
-        <v>394</v>
-      </c>
-      <c r="L55" s="11" t="s">
-        <v>396</v>
+        <v>391</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="L55" s="10" t="s">
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A56" s="22">
+      <c r="A56" s="18">
         <v>58</v>
       </c>
       <c r="B56" s="3" t="s">
@@ -3233,17 +3212,17 @@
         <v>156</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="K56" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="L56" s="11" t="s">
-        <v>398</v>
+        <v>393</v>
+      </c>
+      <c r="K56" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="L56" s="10" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="A57" s="22">
+      <c r="A57" s="18">
         <v>59</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -3256,17 +3235,17 @@
         <v>156</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="K57" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="L57" s="11" t="s">
-        <v>402</v>
+        <v>396</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="L57" s="10" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="A58" s="22">
+      <c r="A58" s="18">
         <v>60</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -3279,13 +3258,13 @@
         <v>156</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="K58" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="L58" s="11" t="s">
-        <v>405</v>
+        <v>399</v>
+      </c>
+      <c r="K58" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="L58" s="10" t="s">
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -3550,7 +3529,7 @@
       <c r="A2" t="s">
         <v>298</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>299</v>
       </c>
       <c r="T2" t="str">
@@ -3562,7 +3541,7 @@
       <c r="A3" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>300</v>
       </c>
       <c r="T3" t="str">
@@ -4009,8 +3988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CD1D2F8-A187-4E57-89FE-37F882500716}">
   <dimension ref="A2:O10"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4023,15 +4002,15 @@
       <c r="A2" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>373</v>
+      <c r="B2" s="17" t="s">
+        <v>382</v>
       </c>
       <c r="C2" s="4" t="str">
         <f>"https://drive.google.com/uc?export=view&amp;id=" &amp; E2</f>
         <v>https://drive.google.com/uc?export=view&amp;id=1INqp-eRs3d5hS5_nlsU4zqYFQkoyYqRl</v>
       </c>
       <c r="D2" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E2" t="str">
         <f>MID(D2,SEARCH("/d/",D2)+3,33)</f>
@@ -4039,22 +4018,22 @@
       </c>
       <c r="O2" s="4" t="str">
         <f>"{title: """&amp;A2&amp;""""&amp;", url: """&amp;B2&amp;""", thumbnail: """ &amp; C2 &amp;"""},"</f>
-        <v>{title: "DOST-Mimaropa, CEST shore up Romblon areas", url: "https://drive.google.com/file/d/1gDnAZMctL5p9RECrUUzC6m2p8q6YkVuP/view?usp=sharing", thumbnail: "https://drive.google.com/uc?export=view&amp;id=1INqp-eRs3d5hS5_nlsU4zqYFQkoyYqRl"},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+        <v>{title: "DOST-Mimaropa, CEST shore up Romblon areas", url: "https://drive.google.com/file/d/1INqp-eRs3d5hS5_nlsU4zqYFQkoyYqRl/view?usp=sharing", thumbnail: "https://drive.google.com/uc?export=view&amp;id=1INqp-eRs3d5hS5_nlsU4zqYFQkoyYqRl"},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>374</v>
+      <c r="B3" s="17" t="s">
+        <v>386</v>
       </c>
       <c r="C3" s="4" t="str">
         <f t="shared" ref="C3:C10" si="0">"https://drive.google.com/uc?export=view&amp;id=" &amp; E3</f>
         <v>https://drive.google.com/uc?export=view&amp;id=1ay4jmlpKpMASeyNnI0_gMY_NBkzZqS9h</v>
       </c>
       <c r="D3" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E10" si="1">MID(D3,SEARCH("/d/",D3)+3,33)</f>
@@ -4062,15 +4041,15 @@
       </c>
       <c r="O3" s="4" t="str">
         <f t="shared" ref="O3:O10" si="2">"{title: """&amp;A3&amp;""""&amp;", url: """&amp;B3&amp;""", thumbnail: """ &amp; C3 &amp;"""},"</f>
-        <v>{title: "Coral restoration in Marinduque begins", url: "https://drive.google.com/file/d/1mnJHmzZ0uBsaE3URHMtPdt6kfnUEj4NM/view?usp=sharing", thumbnail: "https://drive.google.com/uc?export=view&amp;id=1ay4jmlpKpMASeyNnI0_gMY_NBkzZqS9h"},</v>
+        <v>{title: "Coral restoration in Marinduque begins", url: "https://drive.google.com/file/d/1ay4jmlpKpMASeyNnI0_gMY_NBkzZqS9h/view?usp=sharing", thumbnail: "https://drive.google.com/uc?export=view&amp;id=1ay4jmlpKpMASeyNnI0_gMY_NBkzZqS9h"},</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>376</v>
+        <v>373</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>374</v>
       </c>
       <c r="C4" s="4" t="e">
         <f t="shared" si="0"/>
@@ -4089,15 +4068,15 @@
       <c r="A5" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>377</v>
+      <c r="B5" s="17" t="s">
+        <v>375</v>
       </c>
       <c r="C5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>https://drive.google.com/uc?export=view&amp;id=1FMba5lXIw4mekHcyYe9mArir-AFbdErM</v>
       </c>
       <c r="D5" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
@@ -4112,15 +4091,15 @@
       <c r="A6" s="4" t="s">
         <v>308</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>380</v>
+      <c r="B6" s="17" t="s">
+        <v>387</v>
       </c>
       <c r="C6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>https://drive.google.com/uc?export=view&amp;id=1RMDnqHs1VuGLF4VKchjJ6OtsgzYhUSkF</v>
       </c>
       <c r="D6" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
@@ -4128,22 +4107,22 @@
       </c>
       <c r="O6" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>{title: "DoST program extends help to shrimp farmers", url: "https://drive.google.com/file/d/1AfMaBN70wepX_TwY9OOZ5Kw6r9RftlDK/view?usp=sharing", thumbnail: "https://drive.google.com/uc?export=view&amp;id=1RMDnqHs1VuGLF4VKchjJ6OtsgzYhUSkF"},</v>
+        <v>{title: "DoST program extends help to shrimp farmers", url: "https://drive.google.com/file/d/1s4zN1CNVBrut_9hEN0yUwed6O1lpcOWz/view?usp=sharing", thumbnail: "https://drive.google.com/uc?export=view&amp;id=1RMDnqHs1VuGLF4VKchjJ6OtsgzYhUSkF"},</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>378</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>381</v>
       </c>
       <c r="C7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>https://drive.google.com/uc?export=view&amp;id=1s4zN1CNVBrut_9hEN0yUwed6O1lpcOWz</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>391</v>
+      <c r="D7" s="20" t="s">
+        <v>387</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
@@ -4158,15 +4137,15 @@
       <c r="A8" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>382</v>
+      <c r="B8" s="17" t="s">
+        <v>385</v>
       </c>
       <c r="C8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>https://drive.google.com/uc?export=view&amp;id=1a13flG1yKZbT8k2LKiXR16erlc_qFb2w</v>
       </c>
       <c r="D8" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
@@ -4174,15 +4153,15 @@
       </c>
       <c r="O8" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>{title: "DoST to conduct Luzon-wide virtual scientific meeting", url: "https://drive.google.com/file/d/17THWbERvifm5G_Vn6nU2pB6DasYEdI5W/view?usp=sharing", thumbnail: "https://drive.google.com/uc?export=view&amp;id=1a13flG1yKZbT8k2LKiXR16erlc_qFb2w"},</v>
+        <v>{title: "DoST to conduct Luzon-wide virtual scientific meeting", url: "https://drive.google.com/file/d/1a13flG1yKZbT8k2LKiXR16erlc_qFb2w/view?usp=sharing", thumbnail: "https://drive.google.com/uc?export=view&amp;id=1a13flG1yKZbT8k2LKiXR16erlc_qFb2w"},</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>379</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>383</v>
       </c>
       <c r="C9" s="4" t="e">
         <f t="shared" si="0"/>
@@ -4199,10 +4178,10 @@
     </row>
     <row r="10" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C10" s="4" t="e">
         <f t="shared" si="0"/>
@@ -4224,6 +4203,8 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{6B7711E9-4D5D-417C-AA29-0076527169DC}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{E013696A-968E-46D3-8AF0-55586923E666}"/>
     <hyperlink ref="D7" r:id="rId5" xr:uid="{D77F9015-8AC9-487F-9D4F-DA5C214E4C43}"/>
+    <hyperlink ref="B6" r:id="rId6" xr:uid="{E92F88F7-9E94-4EA7-896F-9DB7BF7702AE}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{93690D05-BE13-432E-8F6E-4D3491A293F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4234,7 +4215,7 @@
   <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:M1048576"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4258,7 +4239,7 @@
       <c r="M1" s="2"/>
     </row>
     <row r="43" spans="1:12" ht="300" x14ac:dyDescent="0.25">
-      <c r="A43" s="22">
+      <c r="A43" s="18">
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -4279,15 +4260,15 @@
         <v>276</v>
       </c>
       <c r="J43" s="5"/>
-      <c r="K43" s="10" t="s">
+      <c r="K43" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="L43" s="20" t="s">
+      <c r="L43" s="6" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="285" x14ac:dyDescent="0.25">
-      <c r="A51" s="22">
+      <c r="A51" s="18">
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -4308,15 +4289,15 @@
         <v>287</v>
       </c>
       <c r="J51" s="5"/>
-      <c r="K51" s="17" t="s">
+      <c r="K51" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="L51" s="11" t="s">
+      <c r="L51" s="10" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="300" x14ac:dyDescent="0.25">
-      <c r="A54" s="22">
+      <c r="A54" s="18">
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
@@ -4337,10 +4318,10 @@
         <v>290</v>
       </c>
       <c r="J54" s="5"/>
-      <c r="K54" s="17" t="s">
+      <c r="K54" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="L54" s="11" t="s">
+      <c r="L54" s="10" t="s">
         <v>263</v>
       </c>
     </row>

</xml_diff>